<commit_message>
modified:   Experiment Results/Sarcastic Results.xlsx
</commit_message>
<xml_diff>
--- a/Experiment Results/Sarcastic Results.xlsx
+++ b/Experiment Results/Sarcastic Results.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
   <x:si>
     <x:t xml:space="preserve">ID</x:t>
   </x:si>
@@ -272,6 +272,9 @@
   </x:si>
   <x:si>
     <x:t xml:space="preserve">Chinese</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">MSc</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -368,8 +371,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:AN7" insertRow="1" totalsRowShown="0">
-  <x:autoFilter ref="A1:AN7"/>
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:AN8" insertRow="1" totalsRowShown="0">
+  <x:autoFilter ref="A1:AN8"/>
   <x:tableColumns count="40">
     <x:tableColumn id="1" uniqueName="1" name="ID" dataDxfId="0"/>
     <x:tableColumn id="2" uniqueName="2" name="开始时间" dataDxfId="3"/>
@@ -1601,11 +1604,129 @@
       </x:c>
       <x:c r="AN7" s="10" t="s"/>
     </x:row>
+    <x:row r="8" hidden="0">
+      <x:c r="A8">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="B8" s="2">
+        <x:v>45056.8403125</x:v>
+      </x:c>
+      <x:c r="C8" s="2">
+        <x:v>45056.841412037</x:v>
+      </x:c>
+      <x:c r="D8" s="10" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="E8" s="10" t="s"/>
+      <x:c r="F8" s="10" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="G8" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="H8" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="I8" s="10" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="J8" s="10" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="K8" s="7" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="L8" s="10" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="M8" s="10" t="s">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="N8" s="10" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="O8" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P8" s="10" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="Q8" s="10" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="R8" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="S8" s="10" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="T8" s="10" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="U8" s="10" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="V8" s="10" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="W8">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="X8" s="10" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="Y8" s="7" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="Z8" s="7" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="AA8" s="7" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="AB8" s="7" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="AC8" s="7" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="AD8" s="7" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="AE8" s="7" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="AF8" s="7" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="AG8" s="7" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="AH8" s="7" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="AI8" s="7" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="AJ8" s="7" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="AK8" s="7" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="AL8" s="7" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="AM8" s="7" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="AN8" s="10" t="s"/>
+    </x:row>
   </x:sheetData>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <x:pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <x:tableParts count="1">
-    <x:tablePart r:id="R5b414ea9838d437b"/>
+    <x:tablePart r:id="R9c3f26ee06eb4223"/>
   </x:tableParts>
 </x:worksheet>
 </file>
</xml_diff>